<commit_message>
Improve manchester syntax parsing
</commit_message>
<xml_diff>
--- a/xls2rdf-lib/src/test/resources/suite/_46_manchester/input.xlsx
+++ b/xls2rdf-lib/src/test/resources/suite/_46_manchester/input.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Graph URI</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t xml:space="preserve">ex:Pizza and ex:hasTopping some ex:MeatTopping</t>
+  </si>
+  <si>
+    <t>ex:TEST_DECIMAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:literal_qtt_mg some xsd:decimal[&gt;= 2.5 , &lt;= 3]</t>
   </si>
 </sst>
 </file>
@@ -1163,8 +1169,12 @@
       <c r="C6" s="7"/>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" ht="14.25"/>
     <row r="9" ht="14.25"/>

</xml_diff>